<commit_message>
deleted financial slides from presentation
</commit_message>
<xml_diff>
--- a/Finances/Projections.xlsx
+++ b/Finances/Projections.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tfrancis\OneDrive - Hearst\Documents\Custom Office Templates\dogen\Finances\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="332" documentId="11_376AD7E749603A025F3A1731D194D6F8EB21230F" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{CCA8126D-C73F-4A38-805F-95E6A3904097}"/>
+  <xr:revisionPtr revIDLastSave="335" documentId="11_376AD7E749603A025F3A1731D194D6F8EB21230F" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{39BEFBA9-A1A3-4CE1-9B43-B446F3DDE86E}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="801" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="801" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Directions" sheetId="1" r:id="rId1"/>
@@ -201,7 +201,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -4417,49 +4419,8 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="50" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="43" fontId="50" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="50" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="50" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="50" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="51" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="51" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="54" fillId="7" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="47" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="50" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="50" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="50" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
+    <xf numFmtId="49" fontId="51" fillId="12" borderId="16" xfId="7" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="50" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
@@ -4472,9 +4433,6 @@
     <xf numFmtId="0" fontId="50" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="51" fillId="12" borderId="16" xfId="7" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="51" fillId="12" borderId="16" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -4492,6 +4450,14 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="50" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="43" fontId="50" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="43" fontId="50" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
@@ -4532,6 +4498,42 @@
     </xf>
     <xf numFmtId="0" fontId="47" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="50" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="50" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="50" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="51" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="51" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="54" fillId="7" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="47" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="50" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="50" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="50" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -5571,8 +5573,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="5250179" y="1977390"/>
-          <a:ext cx="2600325" cy="1771651"/>
+          <a:off x="5252084" y="1977390"/>
+          <a:ext cx="2598420" cy="1767841"/>
           <a:chOff x="1525904" y="5981700"/>
           <a:chExt cx="2598420" cy="1767841"/>
         </a:xfrm>
@@ -6755,7 +6757,7 @@
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Key_Assumptions_draft"/>
-      <sheetName val="Community_Engagement"/>
+      <sheetName val="Chart1"/>
       <sheetName val="Revenue_Profit_Balance"/>
       <sheetName val="Funding_And_Connections"/>
       <sheetName val="Comprehensive"/>
@@ -6775,7 +6777,7 @@
       <sheetName val="Eating Area"/>
       <sheetName val="decor"/>
       <sheetName val="Initial"/>
-      <sheetName val="Chart1"/>
+      <sheetName val="Community_Engagement"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0"/>
@@ -6826,11 +6828,6 @@
       </sheetData>
       <sheetData sheetId="9"/>
       <sheetData sheetId="10">
-        <row r="3">
-          <cell r="H3">
-            <v>24.509803921568626</v>
-          </cell>
-        </row>
         <row r="4">
           <cell r="H4">
             <v>22.058823529411764</v>
@@ -7204,8 +7201,8 @@
   </sheetPr>
   <dimension ref="A1:P43"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="18" x14ac:dyDescent="0.5"/>
@@ -7547,7 +7544,7 @@
   </sheetPr>
   <dimension ref="A1:S34"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="80" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScaleNormal="100" zoomScalePageLayoutView="80" workbookViewId="0">
       <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
@@ -8944,7 +8941,7 @@
   </sheetPr>
   <dimension ref="A1:AB33"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="80" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScaleNormal="100" zoomScalePageLayoutView="80" workbookViewId="0">
       <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
@@ -11481,7 +11478,7 @@
   </sheetPr>
   <dimension ref="A1:O67"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="50" workbookViewId="0">
+    <sheetView topLeftCell="A19" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="50" workbookViewId="0">
       <selection activeCell="O60" sqref="O60"/>
     </sheetView>
   </sheetViews>
@@ -14569,7 +14566,7 @@
   </sheetPr>
   <dimension ref="A1:W82"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="70" workbookViewId="0"/>
+    <sheetView topLeftCell="A34" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="70" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.35"/>
   <cols>
@@ -16729,7 +16726,7 @@
   </sheetPr>
   <dimension ref="A1:I47"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
       <selection activeCell="F43" sqref="F43"/>
     </sheetView>
   </sheetViews>
@@ -18584,7 +18581,7 @@
   </sheetPr>
   <dimension ref="A1:H40"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
@@ -19618,7 +19615,7 @@
   <dimension ref="B2:Q159"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="40" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4:G6"/>
+      <selection activeCell="P6" sqref="P6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.35"/>
@@ -25611,7 +25608,7 @@
   </sheetPr>
   <dimension ref="A1:L53"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
       <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
@@ -25641,11 +25638,11 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A2" s="466"/>
-      <c r="B2" s="582" t="s">
+      <c r="B2" s="602" t="s">
         <v>212</v>
       </c>
-      <c r="C2" s="582"/>
-      <c r="D2" s="582"/>
+      <c r="C2" s="602"/>
+      <c r="D2" s="602"/>
       <c r="E2" s="466"/>
       <c r="F2" s="466"/>
       <c r="G2" s="466"/>
@@ -25715,10 +25712,10 @@
       <c r="D7" s="474" t="s">
         <v>159</v>
       </c>
-      <c r="E7" s="590" t="s">
+      <c r="E7" s="578" t="s">
         <v>32</v>
       </c>
-      <c r="F7" s="590"/>
+      <c r="F7" s="578"/>
       <c r="G7" s="475"/>
       <c r="H7" s="466"/>
       <c r="I7" s="466"/>
@@ -25729,8 +25726,8 @@
       <c r="B8" s="476"/>
       <c r="C8" s="477"/>
       <c r="D8" s="477"/>
-      <c r="E8" s="591"/>
-      <c r="F8" s="592"/>
+      <c r="E8" s="579"/>
+      <c r="F8" s="580"/>
       <c r="G8" s="478"/>
       <c r="H8" s="466"/>
       <c r="I8" s="466"/>
@@ -25747,10 +25744,10 @@
       <c r="D9" s="558" t="s">
         <v>354</v>
       </c>
-      <c r="E9" s="593" t="s">
+      <c r="E9" s="581" t="s">
         <v>379</v>
       </c>
-      <c r="F9" s="594"/>
+      <c r="F9" s="582"/>
       <c r="G9" s="478"/>
       <c r="H9" s="466"/>
       <c r="I9" s="466"/>
@@ -25767,10 +25764,10 @@
       <c r="D10" s="482">
         <v>20</v>
       </c>
-      <c r="E10" s="574" t="s">
+      <c r="E10" s="583" t="s">
         <v>379</v>
       </c>
-      <c r="F10" s="575"/>
+      <c r="F10" s="584"/>
       <c r="G10" s="483"/>
       <c r="H10" s="466"/>
       <c r="I10" s="466"/>
@@ -25788,8 +25785,8 @@
       <c r="D11" s="482">
         <v>7</v>
       </c>
-      <c r="E11" s="574"/>
-      <c r="F11" s="575"/>
+      <c r="E11" s="583"/>
+      <c r="F11" s="584"/>
       <c r="G11" s="483"/>
       <c r="H11" s="466"/>
       <c r="I11" s="466"/>
@@ -25807,8 +25804,8 @@
       <c r="D12" s="482">
         <v>7</v>
       </c>
-      <c r="E12" s="574"/>
-      <c r="F12" s="575"/>
+      <c r="E12" s="583"/>
+      <c r="F12" s="584"/>
       <c r="G12" s="483"/>
       <c r="H12" s="466"/>
       <c r="I12" s="466"/>
@@ -25826,8 +25823,8 @@
       <c r="D13" s="482">
         <v>5</v>
       </c>
-      <c r="E13" s="574"/>
-      <c r="F13" s="575"/>
+      <c r="E13" s="583"/>
+      <c r="F13" s="584"/>
       <c r="G13" s="483"/>
       <c r="H13" s="466"/>
       <c r="I13" s="466"/>
@@ -25844,8 +25841,8 @@
       <c r="D14" s="482">
         <v>5</v>
       </c>
-      <c r="E14" s="574"/>
-      <c r="F14" s="575"/>
+      <c r="E14" s="583"/>
+      <c r="F14" s="584"/>
       <c r="G14" s="483"/>
       <c r="H14" s="466"/>
       <c r="I14" s="466"/>
@@ -25862,10 +25859,10 @@
       <c r="D15" s="482">
         <v>5</v>
       </c>
-      <c r="E15" s="574" t="s">
+      <c r="E15" s="583" t="s">
         <v>378</v>
       </c>
-      <c r="F15" s="575"/>
+      <c r="F15" s="584"/>
       <c r="G15" s="483"/>
       <c r="H15" s="466"/>
       <c r="I15" s="466"/>
@@ -25881,8 +25878,8 @@
         <v>83495</v>
       </c>
       <c r="D16" s="486"/>
-      <c r="E16" s="598"/>
-      <c r="F16" s="599"/>
+      <c r="E16" s="588"/>
+      <c r="F16" s="589"/>
       <c r="G16" s="487"/>
       <c r="H16" s="466"/>
       <c r="I16" s="466"/>
@@ -25890,11 +25887,11 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A17" s="466"/>
-      <c r="B17" s="603"/>
-      <c r="C17" s="604"/>
-      <c r="D17" s="604"/>
-      <c r="E17" s="604"/>
-      <c r="F17" s="605"/>
+      <c r="B17" s="593"/>
+      <c r="C17" s="594"/>
+      <c r="D17" s="594"/>
+      <c r="E17" s="594"/>
+      <c r="F17" s="595"/>
       <c r="G17" s="488"/>
       <c r="H17" s="466"/>
       <c r="I17" s="466"/>
@@ -25907,11 +25904,11 @@
       <c r="C18" s="490" t="s">
         <v>1</v>
       </c>
-      <c r="D18" s="595" t="s">
+      <c r="D18" s="585" t="s">
         <v>32</v>
       </c>
-      <c r="E18" s="596"/>
-      <c r="F18" s="597"/>
+      <c r="E18" s="586"/>
+      <c r="F18" s="587"/>
       <c r="G18" s="466"/>
       <c r="H18" s="466"/>
       <c r="I18" s="466"/>
@@ -25924,11 +25921,11 @@
       <c r="C19" s="492">
         <v>0</v>
       </c>
-      <c r="D19" s="576" t="s">
+      <c r="D19" s="596" t="s">
         <v>386</v>
       </c>
-      <c r="E19" s="577"/>
-      <c r="F19" s="578"/>
+      <c r="E19" s="597"/>
+      <c r="F19" s="598"/>
       <c r="G19" s="466"/>
       <c r="H19" s="466"/>
       <c r="I19" s="466"/>
@@ -25941,11 +25938,11 @@
       <c r="C20" s="481">
         <v>5000</v>
       </c>
-      <c r="D20" s="586" t="s">
+      <c r="D20" s="575" t="s">
         <v>381</v>
       </c>
-      <c r="E20" s="587"/>
-      <c r="F20" s="588"/>
+      <c r="E20" s="576"/>
+      <c r="F20" s="577"/>
       <c r="G20" s="466"/>
       <c r="H20" s="466"/>
       <c r="I20" s="466"/>
@@ -25958,11 +25955,11 @@
       <c r="C21" s="481">
         <v>0</v>
       </c>
-      <c r="D21" s="586" t="s">
+      <c r="D21" s="575" t="s">
         <v>382</v>
       </c>
-      <c r="E21" s="587"/>
-      <c r="F21" s="588"/>
+      <c r="E21" s="576"/>
+      <c r="F21" s="577"/>
       <c r="G21" s="466"/>
       <c r="H21" s="466"/>
       <c r="I21" s="466"/>
@@ -25975,11 +25972,11 @@
       <c r="C22" s="481">
         <v>500</v>
       </c>
-      <c r="D22" s="586" t="s">
+      <c r="D22" s="575" t="s">
         <v>380</v>
       </c>
-      <c r="E22" s="587"/>
-      <c r="F22" s="588"/>
+      <c r="E22" s="576"/>
+      <c r="F22" s="577"/>
       <c r="G22" s="466"/>
       <c r="H22" s="466"/>
       <c r="I22" s="466"/>
@@ -25992,11 +25989,11 @@
       <c r="C23" s="481">
         <v>60000</v>
       </c>
-      <c r="D23" s="586" t="s">
+      <c r="D23" s="575" t="s">
         <v>389</v>
       </c>
-      <c r="E23" s="587"/>
-      <c r="F23" s="588"/>
+      <c r="E23" s="576"/>
+      <c r="F23" s="577"/>
       <c r="G23" s="466"/>
       <c r="H23" s="466"/>
       <c r="I23" s="466"/>
@@ -26009,11 +26006,11 @@
       <c r="C24" s="481">
         <v>0</v>
       </c>
-      <c r="D24" s="586" t="s">
+      <c r="D24" s="575" t="s">
         <v>383</v>
       </c>
-      <c r="E24" s="587"/>
-      <c r="F24" s="588"/>
+      <c r="E24" s="576"/>
+      <c r="F24" s="577"/>
       <c r="G24" s="466"/>
       <c r="H24" s="466"/>
       <c r="I24" s="466"/>
@@ -26026,11 +26023,11 @@
       <c r="C25" s="481">
         <v>1000</v>
       </c>
-      <c r="D25" s="586" t="s">
+      <c r="D25" s="575" t="s">
         <v>387</v>
       </c>
-      <c r="E25" s="587"/>
-      <c r="F25" s="588"/>
+      <c r="E25" s="576"/>
+      <c r="F25" s="577"/>
       <c r="G25" s="493"/>
       <c r="H25" s="466"/>
       <c r="I25" s="466"/>
@@ -26043,11 +26040,11 @@
       <c r="C26" s="481">
         <v>5000</v>
       </c>
-      <c r="D26" s="586" t="s">
+      <c r="D26" s="575" t="s">
         <v>388</v>
       </c>
-      <c r="E26" s="587"/>
-      <c r="F26" s="588"/>
+      <c r="E26" s="576"/>
+      <c r="F26" s="577"/>
       <c r="G26" s="466"/>
       <c r="H26" s="466"/>
       <c r="I26" s="466"/>
@@ -26060,11 +26057,11 @@
       <c r="C27" s="481">
         <v>0</v>
       </c>
-      <c r="D27" s="586" t="s">
+      <c r="D27" s="575" t="s">
         <v>384</v>
       </c>
-      <c r="E27" s="587"/>
-      <c r="F27" s="588"/>
+      <c r="E27" s="576"/>
+      <c r="F27" s="577"/>
       <c r="G27" s="466"/>
       <c r="H27" s="466"/>
       <c r="I27" s="466"/>
@@ -26077,11 +26074,11 @@
       <c r="C28" s="481">
         <v>500</v>
       </c>
-      <c r="D28" s="586" t="s">
+      <c r="D28" s="575" t="s">
         <v>385</v>
       </c>
-      <c r="E28" s="587"/>
-      <c r="F28" s="588"/>
+      <c r="E28" s="576"/>
+      <c r="F28" s="577"/>
       <c r="G28" s="466"/>
       <c r="H28" s="466"/>
       <c r="I28" s="466"/>
@@ -26095,11 +26092,11 @@
         <f>[1]Overhead!$B$18</f>
         <v>179983.33333333334</v>
       </c>
-      <c r="D29" s="586" t="s">
+      <c r="D29" s="575" t="s">
         <v>390</v>
       </c>
-      <c r="E29" s="587"/>
-      <c r="F29" s="588"/>
+      <c r="E29" s="576"/>
+      <c r="F29" s="577"/>
       <c r="G29" s="466"/>
       <c r="H29" s="466"/>
       <c r="I29" s="466"/>
@@ -26113,9 +26110,9 @@
         <f>SUM(C19:C29)</f>
         <v>251983.33333333334</v>
       </c>
-      <c r="D30" s="586"/>
-      <c r="E30" s="587"/>
-      <c r="F30" s="588"/>
+      <c r="D30" s="575"/>
+      <c r="E30" s="576"/>
+      <c r="F30" s="577"/>
       <c r="G30" s="466"/>
       <c r="H30" s="466"/>
       <c r="I30" s="466"/>
@@ -26129,9 +26126,9 @@
         <f>C16+C30</f>
         <v>335478.33333333337</v>
       </c>
-      <c r="D31" s="583"/>
-      <c r="E31" s="584"/>
-      <c r="F31" s="585"/>
+      <c r="D31" s="603"/>
+      <c r="E31" s="604"/>
+      <c r="F31" s="605"/>
       <c r="G31" s="466"/>
       <c r="H31" s="466"/>
       <c r="I31" s="466"/>
@@ -26262,11 +26259,11 @@
         <v>0</v>
       </c>
       <c r="H38" s="507"/>
-      <c r="J38" s="581" t="s">
+      <c r="J38" s="601" t="s">
         <v>250</v>
       </c>
-      <c r="K38" s="581"/>
-      <c r="L38" s="581"/>
+      <c r="K38" s="601"/>
+      <c r="L38" s="601"/>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A39" s="466"/>
@@ -26289,9 +26286,9 @@
         <v>0</v>
       </c>
       <c r="H39" s="507"/>
-      <c r="J39" s="581"/>
-      <c r="K39" s="581"/>
-      <c r="L39" s="581"/>
+      <c r="J39" s="601"/>
+      <c r="K39" s="601"/>
+      <c r="L39" s="601"/>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A40" s="466"/>
@@ -26314,9 +26311,9 @@
         <v>0</v>
       </c>
       <c r="H40" s="507"/>
-      <c r="J40" s="581"/>
-      <c r="K40" s="581"/>
-      <c r="L40" s="581"/>
+      <c r="J40" s="601"/>
+      <c r="K40" s="601"/>
+      <c r="L40" s="601"/>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A41" s="466"/>
@@ -26339,9 +26336,9 @@
         <v>0</v>
       </c>
       <c r="H41" s="512"/>
-      <c r="J41" s="581"/>
-      <c r="K41" s="581"/>
-      <c r="L41" s="581"/>
+      <c r="J41" s="601"/>
+      <c r="K41" s="601"/>
+      <c r="L41" s="601"/>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A42" s="466"/>
@@ -26356,10 +26353,10 @@
         <f>SUM(D34:D41)</f>
         <v>335478.33333333337</v>
       </c>
-      <c r="E42" s="579" t="s">
+      <c r="E42" s="599" t="s">
         <v>261</v>
       </c>
-      <c r="F42" s="580"/>
+      <c r="F42" s="600"/>
       <c r="G42" s="514">
         <f>SUM(G37:G41)</f>
         <v>0</v>
@@ -26376,12 +26373,12 @@
         <f>C31-D42</f>
         <v>0</v>
       </c>
-      <c r="E43" s="600" t="str">
+      <c r="E43" s="590" t="str">
         <f>IF(D43&gt;0,"You require more funding (Not Balanced)",IF(D43&lt;0,"Your funding exceeds your needs (Not Balanced)","You are fully funded (Balanced)"))</f>
         <v>You are fully funded (Balanced)</v>
       </c>
-      <c r="F43" s="601"/>
-      <c r="G43" s="602"/>
+      <c r="F43" s="591"/>
+      <c r="G43" s="592"/>
       <c r="H43" s="516"/>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.45">
@@ -26407,10 +26404,10 @@
       <c r="H45" s="466"/>
     </row>
     <row r="46" spans="1:12" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B46" s="589" t="s">
+      <c r="B46" s="574" t="s">
         <v>232</v>
       </c>
-      <c r="C46" s="589"/>
+      <c r="C46" s="574"/>
       <c r="D46" s="519"/>
       <c r="E46" s="519"/>
       <c r="F46" s="519"/>
@@ -26488,6 +26485,20 @@
   </sheetData>
   <sheetProtection password="CC3D" sheet="1" objects="1" scenarios="1" formatColumns="0" formatRows="0"/>
   <mergeCells count="30">
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="D19:F19"/>
+    <mergeCell ref="E42:F42"/>
+    <mergeCell ref="J38:L41"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="D31:F31"/>
+    <mergeCell ref="D22:F22"/>
+    <mergeCell ref="D20:F20"/>
+    <mergeCell ref="D21:F21"/>
+    <mergeCell ref="D26:F26"/>
+    <mergeCell ref="D25:F25"/>
+    <mergeCell ref="D24:F24"/>
+    <mergeCell ref="D23:F23"/>
+    <mergeCell ref="D29:F29"/>
     <mergeCell ref="B46:C46"/>
     <mergeCell ref="D27:F27"/>
     <mergeCell ref="D28:F28"/>
@@ -26504,20 +26515,6 @@
     <mergeCell ref="B17:F17"/>
     <mergeCell ref="E14:F14"/>
     <mergeCell ref="D30:F30"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="D19:F19"/>
-    <mergeCell ref="E42:F42"/>
-    <mergeCell ref="J38:L41"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="D31:F31"/>
-    <mergeCell ref="D22:F22"/>
-    <mergeCell ref="D20:F20"/>
-    <mergeCell ref="D21:F21"/>
-    <mergeCell ref="D26:F26"/>
-    <mergeCell ref="D25:F25"/>
-    <mergeCell ref="D24:F24"/>
-    <mergeCell ref="D23:F23"/>
-    <mergeCell ref="D29:F29"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="C9:C15 C19:C29 D34:D35 D37:D41">
@@ -26563,7 +26560,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
@@ -26723,7 +26720,7 @@
   </sheetPr>
   <dimension ref="A1:R32"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="50" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScaleNormal="100" zoomScalePageLayoutView="50" workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
@@ -29427,7 +29424,7 @@
   </sheetPr>
   <dimension ref="A1:S60"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScaleNormal="100" zoomScalePageLayoutView="50" workbookViewId="0">
+    <sheetView topLeftCell="A13" zoomScaleNormal="100" zoomScalePageLayoutView="50" workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
@@ -31797,8 +31794,8 @@
   </sheetPr>
   <dimension ref="A1:AF49"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" zoomScaleNormal="100" zoomScalePageLayoutView="50" workbookViewId="0">
-      <selection activeCell="A50" sqref="A50"/>
+    <sheetView topLeftCell="M8" zoomScaleNormal="100" zoomScalePageLayoutView="50" workbookViewId="0">
+      <selection activeCell="S18" sqref="S18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.35"/>
@@ -31812,7 +31809,7 @@
     <col min="7" max="7" width="9.44140625" style="63" customWidth="1"/>
     <col min="8" max="8" width="9" style="71" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9.33203125" style="71" customWidth="1"/>
-    <col min="10" max="10" width="9" style="71" customWidth="1"/>
+    <col min="10" max="10" width="10.33203125" style="71" customWidth="1"/>
     <col min="11" max="11" width="11.88671875" style="71" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="9" style="71" bestFit="1" customWidth="1"/>
     <col min="13" max="14" width="11.33203125" style="71" bestFit="1" customWidth="1"/>
@@ -31821,7 +31818,8 @@
     <col min="17" max="17" width="11.33203125" style="71" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="8.88671875" style="71"/>
     <col min="19" max="19" width="10.33203125" style="71" bestFit="1" customWidth="1"/>
-    <col min="20" max="25" width="8.88671875" style="71"/>
+    <col min="20" max="24" width="8.88671875" style="71"/>
+    <col min="25" max="25" width="9.88671875" style="71" customWidth="1"/>
     <col min="26" max="26" width="11.88671875" style="71" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="9.5546875" style="71" bestFit="1" customWidth="1"/>
     <col min="28" max="29" width="11.33203125" style="71" bestFit="1" customWidth="1"/>
@@ -36116,7 +36114,7 @@
   </sheetPr>
   <dimension ref="A1:R45"/>
   <sheetViews>
-    <sheetView topLeftCell="G19" zoomScaleNormal="100" zoomScalePageLayoutView="50" workbookViewId="0">
+    <sheetView topLeftCell="A13" zoomScaleNormal="100" zoomScalePageLayoutView="50" workbookViewId="0">
       <selection activeCell="R35" sqref="R35"/>
     </sheetView>
   </sheetViews>
@@ -36826,8 +36824,8 @@
   </sheetPr>
   <dimension ref="A1:R38"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView topLeftCell="A4" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
+      <selection activeCell="M30" sqref="M30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.35"/>

</xml_diff>